<commit_message>
Completes system for aggregate end-use with ref tech
</commit_message>
<xml_diff>
--- a/gcam-data-system/_common/documentation/Data_system_structure.xlsx
+++ b/gcam-data-system/_common/documentation/Data_system_structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15900" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
   <si>
     <t>01</t>
   </si>
@@ -301,15 +301,6 @@
     <t>323</t>
   </si>
   <si>
-    <t>Cement</t>
-  </si>
-  <si>
-    <t>Buildings</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
     <t>Fossil resources</t>
   </si>
   <si>
@@ -364,43 +355,85 @@
     <t>Downscaling of all data</t>
   </si>
   <si>
-    <t>End-use sectors</t>
-  </si>
-  <si>
     <t>General end use sectors</t>
   </si>
   <si>
-    <t>Placeholder for iron and steel</t>
-  </si>
-  <si>
-    <t>N Fertilizer</t>
-  </si>
-  <si>
-    <t>Detailed regional industrial sectors</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
     <t>China</t>
   </si>
   <si>
-    <t>Brazil</t>
-  </si>
-  <si>
     <t>Detailed regional buildings sectors</t>
   </si>
   <si>
-    <t>351</t>
-  </si>
-  <si>
-    <t>3311</t>
-  </si>
-  <si>
-    <t>3321</t>
-  </si>
-  <si>
-    <t>3331</t>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Buildings: box that consumes energy</t>
+  </si>
+  <si>
+    <t>GCAM 3.0 buildings</t>
+  </si>
+  <si>
+    <t>HDD/CDD</t>
+  </si>
+  <si>
+    <t>50s</t>
+  </si>
+  <si>
+    <t>Transportation: box that consumes energy</t>
+  </si>
+  <si>
+    <t>GCAM 3.0 transportation</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>UCD transportation</t>
+  </si>
+  <si>
+    <t>331</t>
+  </si>
+  <si>
+    <t>332</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>Detailed sector: cement</t>
+  </si>
+  <si>
+    <t>Detailed sector: N fertilizer</t>
+  </si>
+  <si>
+    <t>Detailed sector: iron and steel</t>
+  </si>
+  <si>
+    <t>Detailed region: USA</t>
+  </si>
+  <si>
+    <t>Detailed region: China</t>
+  </si>
+  <si>
+    <t>Detailed region: Brazil</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>451</t>
+  </si>
+  <si>
+    <t>452</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
   </si>
 </sst>
 </file>
@@ -461,8 +494,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -552,7 +597,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -593,6 +638,12 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -633,6 +684,12 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -962,17 +1019,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -986,10 +1043,10 @@
     <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1005,7 +1062,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1022,7 +1079,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1031,7 +1088,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1040,7 +1097,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -1050,7 +1107,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1059,7 +1116,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1068,7 +1125,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1085,7 +1142,7 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1104,7 +1161,7 @@
         <v>40</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1114,7 +1171,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1124,7 +1181,7 @@
         <v>42</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1134,7 +1191,7 @@
         <v>43</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1144,7 +1201,7 @@
         <v>44</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1163,7 +1220,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1190,7 +1247,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1198,7 +1255,7 @@
         <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1207,7 +1264,7 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1225,7 +1282,7 @@
         <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1234,7 +1291,7 @@
         <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1243,79 +1300,121 @@
         <v>92</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C34" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" t="s">
-        <v>120</v>
-      </c>
+      <c r="A35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="1"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="B39" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="B41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="B43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="B44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" t="s">
         <v>123</v>
-      </c>
-      <c r="C38" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
entire module w/aggregate sectors exc cement and fert; start of global detailed bld
</commit_message>
<xml_diff>
--- a/gcam-data-system/_common/documentation/Data_system_structure.xlsx
+++ b/gcam-data-system/_common/documentation/Data_system_structure.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="140">
   <si>
     <t>01</t>
   </si>
@@ -434,6 +434,12 @@
   </si>
   <si>
     <t>54</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Traditional biomass</t>
   </si>
 </sst>
 </file>
@@ -1019,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1129,291 +1135,300 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>102</v>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>107</v>
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" t="s">
-        <v>39</v>
+        <v>20</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>127</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1"/>
-      <c r="B31" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>129</v>
+      <c r="B31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" t="s">
-        <v>130</v>
+      <c r="B32" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" t="s">
-        <v>116</v>
-      </c>
+      <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="B39" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C39" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="B40" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="B41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="B42" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="B43" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C43" t="s">
-        <v>120</v>
-      </c>
+      <c r="B43" s="1"/>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cement and other calibration adjustments
</commit_message>
<xml_diff>
--- a/gcam-data-system/_common/documentation/Data_system_structure.xlsx
+++ b/gcam-data-system/_common/documentation/Data_system_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="260" yWindow="20" windowWidth="33780" windowHeight="19040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="energy" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="171">
   <si>
     <t>01</t>
   </si>
@@ -440,6 +440,99 @@
   </si>
   <si>
     <t>Traditional biomass</t>
+  </si>
+  <si>
+    <t>historical floorspace</t>
+  </si>
+  <si>
+    <t>satiation of floorspace</t>
+  </si>
+  <si>
+    <t>satiation of services</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>processed from other sources</t>
+  </si>
+  <si>
+    <t>assumed</t>
+  </si>
+  <si>
+    <t>price elasticity of floorspace</t>
+  </si>
+  <si>
+    <t>degree days</t>
+  </si>
+  <si>
+    <t>processed by Yuyu (GIS)</t>
+  </si>
+  <si>
+    <t>processed from base year data, multiplied by exog multipliers and other adjustments</t>
+  </si>
+  <si>
+    <t>non-US regions: heating and cooling satiation levels equal to US base-year level, multiplied by HDD or CDD ratio</t>
+  </si>
+  <si>
+    <t>internal gain scaler</t>
+  </si>
+  <si>
+    <t>exogenous (set to artificially low level in order to nullify potentially negative impacts of this parameter)</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>service output ("base service")</t>
+  </si>
+  <si>
+    <t>aggregated as the sum of all service outputs (at the tech level)</t>
+  </si>
+  <si>
+    <t>shell conductance</t>
+  </si>
+  <si>
+    <t>USA: US input set. Other regions: assigned exogenous tech change</t>
+  </si>
+  <si>
+    <t>fuel preference elasticity</t>
+  </si>
+  <si>
+    <t>efficiency</t>
+  </si>
+  <si>
+    <t>usa from detailed US data. Other regions multiplied by exogenous region- and time-specific adjustment factors</t>
+  </si>
+  <si>
+    <t>callibrated energy consumption</t>
+  </si>
+  <si>
+    <t>IEA energy balances' building energy demand by fuel, multiplied by service allocation shares</t>
+  </si>
+  <si>
+    <t>service allocation shares</t>
+  </si>
+  <si>
+    <t>requires processing; from specific data sources for countries and regions</t>
+  </si>
+  <si>
+    <t>non-fuel costs</t>
+  </si>
+  <si>
+    <t>calculated from exogenous assumptions about capital costs, interest rates, O&amp;M costs, UECs, and efficiencies of each technology</t>
+  </si>
+  <si>
+    <t>internal load fraction</t>
+  </si>
+  <si>
+    <t>exogenous (equal for all techs right now)</t>
+  </si>
+  <si>
+    <t>retirement</t>
+  </si>
+  <si>
+    <t>exogenous (from USA data processing)</t>
   </si>
 </sst>
 </file>
@@ -500,8 +593,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -603,7 +700,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -650,6 +747,8 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -696,6 +795,8 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1025,13 +1126,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1318,7 +1422,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:11">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>124</v>
@@ -1327,7 +1431,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:11">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>125</v>
@@ -1335,8 +1439,14 @@
       <c r="C34" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="J34" t="s">
+        <v>153</v>
+      </c>
+      <c r="K34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>126</v>
@@ -1344,14 +1454,26 @@
       <c r="C35" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="J35" t="s">
+        <v>140</v>
+      </c>
+      <c r="K35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="J36" t="s">
+        <v>141</v>
+      </c>
+      <c r="K36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>30</v>
@@ -1359,8 +1481,14 @@
       <c r="C37" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="J37" t="s">
+        <v>146</v>
+      </c>
+      <c r="K37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>31</v>
@@ -1368,8 +1496,14 @@
       <c r="C38" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="J38" t="s">
+        <v>147</v>
+      </c>
+      <c r="K38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
         <v>51</v>
@@ -1377,59 +1511,136 @@
       <c r="C39" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="J39" t="s">
+        <v>142</v>
+      </c>
+      <c r="K39" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="B40" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C40" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="K40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="B41" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C41" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="J41" t="s">
+        <v>151</v>
+      </c>
+      <c r="K41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="B42" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C42" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="J42" t="s">
+        <v>154</v>
+      </c>
+      <c r="K42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="J43" t="s">
+        <v>156</v>
+      </c>
+      <c r="K43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="B44" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C44" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="J44" t="s">
+        <v>158</v>
+      </c>
+      <c r="K44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="B45" s="1" t="s">
         <v>136</v>
       </c>
       <c r="C45" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="J45" t="s">
+        <v>159</v>
+      </c>
+      <c r="K45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="B46" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C46" t="s">
         <v>123</v>
+      </c>
+      <c r="J46" t="s">
+        <v>161</v>
+      </c>
+      <c r="K46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="J47" t="s">
+        <v>163</v>
+      </c>
+      <c r="K47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="J48" t="s">
+        <v>165</v>
+      </c>
+      <c r="K48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="10:11">
+      <c r="J49" t="s">
+        <v>167</v>
+      </c>
+      <c r="K49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="10:11">
+      <c r="J50" t="s">
+        <v>169</v>
+      </c>
+      <c r="K50" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
includes carbon storage curves and associated info
</commit_message>
<xml_diff>
--- a/gcam-data-system/_common/documentation/Data_system_structure.xlsx
+++ b/gcam-data-system/_common/documentation/Data_system_structure.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="176">
   <si>
     <t>01</t>
   </si>
@@ -533,6 +533,21 @@
   </si>
   <si>
     <t>exogenous (from USA data processing)</t>
+  </si>
+  <si>
+    <t>60s</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>Carbon storage</t>
+  </si>
+  <si>
+    <t>Buildings</t>
+  </si>
+  <si>
+    <t>Transportation</t>
   </si>
 </sst>
 </file>
@@ -1128,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1465,7 +1480,9 @@
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="J36" t="s">
         <v>141</v>
       </c>
@@ -1561,7 +1578,9 @@
       <c r="A43" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>175</v>
+      </c>
       <c r="J43" t="s">
         <v>156</v>
       </c>
@@ -1612,6 +1631,12 @@
       </c>
     </row>
     <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>171</v>
+      </c>
+      <c r="B47" t="s">
+        <v>173</v>
+      </c>
       <c r="J47" t="s">
         <v>163</v>
       </c>
@@ -1620,6 +1645,12 @@
       </c>
     </row>
     <row r="48" spans="1:11">
+      <c r="B48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C48" t="s">
+        <v>173</v>
+      </c>
       <c r="J48" t="s">
         <v>165</v>
       </c>

</xml_diff>